<commit_message>
small fixes, Jenn Phone #, Scheels address line
</commit_message>
<xml_diff>
--- a/assets/Chewy/Chewy UCC128 Label Request - Copy.xlsx
+++ b/assets/Chewy/Chewy UCC128 Label Request - Copy.xlsx
@@ -137,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,14 +148,20 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -302,12 +308,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -394,8 +400,8 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -404,13 +410,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -734,8 +743,8 @@
     <col min="9" max="9" style="34" width="26.862142857142857" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="37" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="37" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="37" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="37" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="38" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="38" width="10.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -770,7 +779,7 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -793,7 +802,7 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -877,7 +886,7 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
@@ -1023,7 +1032,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="26"/>
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>

</xml_diff>